<commit_message>
use PS64 to resolve Rydbergs, add denser model
These adjust the number of l-resolved shells according to
the figure in PS.  Also add denser model, log n =8.

The ratios in the spreadsheet are today/Porter and
they are much much better at lower densities.
There are major differences in 10830 due to
the LS CS bug Giulio found (those cells have a
red tint) and the strong diagnostic lines have a
yellow tint.  Those are good at low densities and
diverge at higher density, probably due to the different
n-changing collision theory we now use.
</commit_message>
<xml_diff>
--- a/tsuite/experimental/he1nnt4.xlsx
+++ b/tsuite/experimental/he1nnt4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gary/Dropbox/papers/Guzman_HeI/21_Porter_redo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gary/cloudy/branches/CaseB22/tsuite/experimental/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD4130B-E4DD-0E4F-A9B0-54391B5BC5E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87EABD8-F695-D042-AC3D-6ED08BBBEAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3800" yWindow="3920" windowWidth="27640" windowHeight="16940" xr2:uid="{8843D32E-1EA8-8F49-A1DE-0F59999A652D}"/>
+    <workbookView xWindow="12500" yWindow="5320" windowWidth="27640" windowHeight="16940" xr2:uid="{8843D32E-1EA8-8F49-A1DE-0F59999A652D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="50">
   <si>
     <t>#lineslist</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>Blnd = triooplet, full multiplet</t>
+  </si>
+  <si>
+    <t>T=4/n=8</t>
   </si>
 </sst>
 </file>
@@ -203,15 +206,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -248,11 +263,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -261,6 +285,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8986F502-92BC-724D-9F3B-72E4E784D06A}">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -587,9 +619,10 @@
     <col min="3" max="3" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>43</v>
@@ -602,18 +635,22 @@
       <c r="F1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="6" t="s">
+      <c r="G1" s="6"/>
+      <c r="H1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="I1" s="9"/>
+      <c r="J1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
+    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="B2" s="2"/>
       <c r="C2" t="s">
         <v>0</v>
@@ -627,8 +664,11 @@
         <v>0</v>
       </c>
       <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>45</v>
       </c>
@@ -641,1051 +681,1294 @@
       <c r="G3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>1.0367</v>
+        <v>1.0013000000000001</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="1">
-        <v>1.0342</v>
+        <v>1.0044</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
       </c>
       <c r="F4" s="1">
-        <v>1.0173000000000001</v>
+        <v>1.0011000000000001</v>
       </c>
       <c r="G4" t="s">
         <v>1</v>
       </c>
       <c r="H4" s="1">
-        <v>0.99187000000000003</v>
-      </c>
-      <c r="J4" t="s">
+        <v>1.0067999999999999</v>
+      </c>
+      <c r="I4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.97755999999999998</v>
+      </c>
+      <c r="K4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>1.0346</v>
+        <v>1.0004</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="1">
-        <v>1.0304</v>
+        <v>1.002</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
       </c>
       <c r="F5" s="1">
-        <v>0.98414000000000001</v>
+        <v>0.96838000000000002</v>
       </c>
       <c r="G5" t="s">
         <v>2</v>
       </c>
       <c r="H5" s="1">
-        <v>0.94862999999999997</v>
-      </c>
-      <c r="J5" t="s">
+        <v>0.96111999999999997</v>
+      </c>
+      <c r="I5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.92247000000000001</v>
+      </c>
+      <c r="K5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="1">
-        <v>1.0288999999999999</v>
+        <v>1.0007999999999999</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="1">
-        <v>1.0269999999999999</v>
+        <v>1.0037</v>
       </c>
       <c r="E6" t="s">
         <v>3</v>
       </c>
       <c r="F6" s="1">
-        <v>1.0119</v>
+        <v>1.0006999999999999</v>
       </c>
       <c r="G6" t="s">
         <v>3</v>
       </c>
       <c r="H6" s="1">
-        <v>0.98936999999999997</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0.99983</v>
+      </c>
+      <c r="I6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.95409999999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1">
-        <v>1.0306999999999999</v>
+        <v>1.0004</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="1">
-        <v>1.0269999999999999</v>
+        <v>1.002</v>
       </c>
       <c r="E7" t="s">
         <v>4</v>
       </c>
       <c r="F7" s="1">
-        <v>0.98723000000000005</v>
+        <v>0.97352000000000005</v>
       </c>
       <c r="G7" t="s">
         <v>4</v>
       </c>
       <c r="H7" s="1">
-        <v>0.95462999999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0.96538999999999997</v>
+      </c>
+      <c r="I7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.92059000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="1">
-        <v>0.99941000000000002</v>
+        <v>1.0004</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="1">
-        <v>0.99773999999999996</v>
+        <v>1.0002</v>
       </c>
       <c r="E8" t="s">
         <v>5</v>
       </c>
       <c r="F8" s="1">
-        <v>0.98453999999999997</v>
+        <v>0.98877999999999999</v>
       </c>
       <c r="G8" t="s">
         <v>5</v>
       </c>
       <c r="H8" s="1">
-        <v>0.96516999999999997</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0.96291000000000004</v>
+      </c>
+      <c r="I8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.90178999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="1">
-        <v>0.98104999999999998</v>
+        <v>0.99914000000000003</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="1">
-        <v>0.98141</v>
+        <v>0.99853999999999998</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
       </c>
       <c r="F9" s="1">
-        <v>0.98314000000000001</v>
+        <v>0.99365000000000003</v>
       </c>
       <c r="G9" t="s">
         <v>6</v>
       </c>
       <c r="H9" s="1">
-        <v>0.97940000000000005</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0.97019</v>
+      </c>
+      <c r="I9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.91574999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="1">
-        <v>1.0008999999999999</v>
+        <v>0.99982000000000004</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="1">
-        <v>0.99814000000000003</v>
+        <v>0.99875999999999998</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="1">
-        <v>0.9627</v>
+        <v>0.96452000000000004</v>
       </c>
       <c r="G10" t="s">
         <v>7</v>
       </c>
       <c r="H10" s="1">
-        <v>0.93638999999999994</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0.93418999999999996</v>
+      </c>
+      <c r="I10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.86551999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="1">
-        <v>0.98806000000000005</v>
+        <v>0.99912000000000001</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="1">
-        <v>0.98607999999999996</v>
+        <v>0.99827999999999995</v>
       </c>
       <c r="E11" t="s">
         <v>8</v>
       </c>
       <c r="F11" s="1">
-        <v>0.96319999999999995</v>
+        <v>0.97172999999999998</v>
       </c>
       <c r="G11" t="s">
         <v>8</v>
       </c>
       <c r="H11" s="1">
-        <v>0.95481000000000005</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+        <v>0.94496999999999998</v>
+      </c>
+      <c r="I11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.89856999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="1">
-        <v>0.98641999999999996</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B12" s="11">
+        <v>0.99980000000000002</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="1">
-        <v>0.98521000000000003</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="D12" s="11">
+        <v>0.99804999999999999</v>
+      </c>
+      <c r="E12" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="1">
-        <v>0.97140000000000004</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="F12" s="11">
+        <v>0.98163999999999996</v>
+      </c>
+      <c r="G12" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="1">
-        <v>0.95213000000000003</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H12" s="11">
+        <v>0.94701000000000002</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" s="11">
+        <v>0.88202999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="1">
-        <v>0.98882000000000003</v>
+        <v>0.99909999999999999</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="1">
-        <v>0.98907</v>
+        <v>0.99941000000000002</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="1">
-        <v>0.98875999999999997</v>
+        <v>0.99534</v>
       </c>
       <c r="G13" t="s">
         <v>10</v>
       </c>
       <c r="H13" s="1">
-        <v>0.98143000000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0.97572999999999999</v>
+      </c>
+      <c r="I13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0.90586999999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="1">
-        <v>0.9859</v>
+        <v>0.99934999999999996</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="1">
-        <v>0.98346999999999996</v>
+        <v>0.99628000000000005</v>
       </c>
       <c r="E14" t="s">
         <v>11</v>
       </c>
       <c r="F14" s="1">
-        <v>0.94266000000000005</v>
+        <v>0.95109999999999995</v>
       </c>
       <c r="G14" t="s">
         <v>11</v>
       </c>
       <c r="H14" s="1">
-        <v>0.91703999999999997</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0.91056999999999999</v>
+      </c>
+      <c r="I14" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0.84523999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="1">
-        <v>1.0223</v>
+        <v>1.0002</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="1">
-        <v>1.0189999999999999</v>
+        <v>1.0012000000000001</v>
       </c>
       <c r="E15" t="s">
         <v>12</v>
       </c>
       <c r="F15" s="1">
-        <v>0.98323000000000005</v>
+        <v>0.97394000000000003</v>
       </c>
       <c r="G15" t="s">
         <v>12</v>
       </c>
       <c r="H15" s="1">
-        <v>0.95411999999999997</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0.96128999999999998</v>
+      </c>
+      <c r="I15" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0.91208999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="1">
-        <v>0.99341999999999997</v>
+        <v>0.99909999999999999</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="1">
-        <v>0.99131999999999998</v>
+        <v>0.99868000000000001</v>
       </c>
       <c r="E16" t="s">
         <v>13</v>
       </c>
       <c r="F16" s="1">
-        <v>0.96562000000000003</v>
+        <v>0.97109999999999996</v>
       </c>
       <c r="G16" t="s">
         <v>13</v>
       </c>
       <c r="H16" s="1">
-        <v>0.95398000000000005</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+        <v>0.94703999999999999</v>
+      </c>
+      <c r="I16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0.89078000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="1">
-        <v>0.93613000000000002</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B17" s="11">
+        <v>0.99644999999999995</v>
+      </c>
+      <c r="C17" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="1">
-        <v>0.93783000000000005</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="D17" s="11">
+        <v>0.98763999999999996</v>
+      </c>
+      <c r="E17" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="1">
-        <v>0.92452999999999996</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="F17" s="11">
+        <v>0.95392999999999994</v>
+      </c>
+      <c r="G17" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H17" s="1">
-        <v>0.91142999999999996</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="H17" s="11">
+        <v>0.89798</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" s="11">
+        <v>0.82025999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="1">
-        <v>0.93396999999999997</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="B18" s="11">
+        <v>0.99648999999999999</v>
+      </c>
+      <c r="C18" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="1">
-        <v>0.93318999999999996</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="D18" s="11">
+        <v>0.98460999999999999</v>
+      </c>
+      <c r="E18" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="1">
-        <v>0.86616000000000004</v>
-      </c>
-      <c r="G18" t="s">
+      <c r="F18" s="11">
+        <v>0.89251000000000003</v>
+      </c>
+      <c r="G18" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="1">
-        <v>0.84950000000000003</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H18" s="11">
+        <v>0.83191999999999999</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J18" s="11">
+        <v>0.78088000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="1">
-        <v>1.0005999999999999</v>
+        <v>0.99702000000000002</v>
       </c>
       <c r="C19" t="s">
         <v>16</v>
       </c>
       <c r="D19" s="1">
-        <v>1.0025999999999999</v>
+        <v>1.0008999999999999</v>
       </c>
       <c r="E19" t="s">
         <v>16</v>
       </c>
       <c r="F19" s="1">
-        <v>1.0015000000000001</v>
+        <v>1.0017</v>
       </c>
       <c r="G19" t="s">
         <v>16</v>
       </c>
       <c r="H19" s="1">
-        <v>0.98916999999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.98911000000000004</v>
+      </c>
+      <c r="I19" t="s">
+        <v>16</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0.90383999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="1">
-        <v>1.0011000000000001</v>
+        <v>0.99855000000000005</v>
       </c>
       <c r="C20" t="s">
         <v>17</v>
       </c>
       <c r="D20" s="1">
-        <v>0.99936000000000003</v>
+        <v>0.99931999999999999</v>
       </c>
       <c r="E20" t="s">
         <v>17</v>
       </c>
       <c r="F20" s="1">
-        <v>0.97577999999999998</v>
+        <v>0.97687999999999997</v>
       </c>
       <c r="G20" t="s">
         <v>17</v>
       </c>
       <c r="H20" s="1">
-        <v>0.96155000000000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.95899000000000001</v>
+      </c>
+      <c r="I20" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0.90114000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B21" s="1">
-        <v>1.0403</v>
+        <v>1.0014000000000001</v>
       </c>
       <c r="C21" t="s">
         <v>18</v>
       </c>
       <c r="D21" s="1">
-        <v>1.0375000000000001</v>
+        <v>1.0045999999999999</v>
       </c>
       <c r="E21" t="s">
         <v>18</v>
       </c>
       <c r="F21" s="1">
-        <v>1.0183</v>
+        <v>0.99956999999999996</v>
       </c>
       <c r="G21" t="s">
         <v>18</v>
       </c>
       <c r="H21" s="1">
-        <v>0.99043000000000003</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+        <v>1.008</v>
+      </c>
+      <c r="I21" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0.98345000000000005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="1">
-        <v>0.97616000000000003</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="B22" s="14">
+        <v>0.97904999999999998</v>
+      </c>
+      <c r="C22" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="1">
-        <v>0.89710999999999996</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="D22" s="14">
+        <v>0.89902000000000004</v>
+      </c>
+      <c r="E22" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F22" s="1">
-        <v>0.52837000000000001</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="F22" s="14">
+        <v>0.52868000000000004</v>
+      </c>
+      <c r="G22" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="H22" s="1">
-        <v>0.50273000000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H22" s="14">
+        <v>0.50312999999999997</v>
+      </c>
+      <c r="I22" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" s="14">
+        <v>0.43336000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="1">
-        <v>1.0346</v>
+        <v>1.0004</v>
       </c>
       <c r="C23" t="s">
         <v>20</v>
       </c>
       <c r="D23" s="1">
-        <v>1.0304</v>
+        <v>1.002</v>
       </c>
       <c r="E23" t="s">
         <v>20</v>
       </c>
       <c r="F23" s="1">
-        <v>0.98412999999999995</v>
+        <v>0.96836999999999995</v>
       </c>
       <c r="G23" t="s">
         <v>20</v>
       </c>
       <c r="H23" s="1">
-        <v>0.94862000000000002</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.96111000000000002</v>
+      </c>
+      <c r="I23" t="s">
+        <v>20</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0.92245999999999995</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="1">
-        <v>0.99943000000000004</v>
+        <v>1.0004</v>
       </c>
       <c r="C24" t="s">
         <v>21</v>
       </c>
       <c r="D24" s="1">
-        <v>0.99773000000000001</v>
+        <v>1.0002</v>
       </c>
       <c r="E24" t="s">
         <v>21</v>
       </c>
       <c r="F24" s="1">
-        <v>0.98453000000000002</v>
+        <v>0.98877999999999999</v>
       </c>
       <c r="G24" t="s">
         <v>21</v>
       </c>
       <c r="H24" s="1">
-        <v>0.96516000000000002</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.96289999999999998</v>
+      </c>
+      <c r="I24" t="s">
+        <v>21</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0.90178999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B25" s="1">
-        <v>1.0367</v>
+        <v>1.0013000000000001</v>
       </c>
       <c r="C25" t="s">
         <v>22</v>
       </c>
       <c r="D25" s="1">
-        <v>1.0342</v>
+        <v>1.0044</v>
       </c>
       <c r="E25" t="s">
         <v>22</v>
       </c>
       <c r="F25" s="1">
-        <v>1.0173000000000001</v>
+        <v>1.0011000000000001</v>
       </c>
       <c r="G25" t="s">
         <v>22</v>
       </c>
       <c r="H25" s="1">
-        <v>0.99187000000000003</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1.0067999999999999</v>
+      </c>
+      <c r="I25" t="s">
+        <v>22</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0.97755999999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B26" s="1">
-        <v>0.92764999999999997</v>
+        <v>0.99765000000000004</v>
       </c>
       <c r="C26" t="s">
         <v>23</v>
       </c>
       <c r="D26" s="1">
-        <v>0.92800000000000005</v>
+        <v>0.98875000000000002</v>
       </c>
       <c r="E26" t="s">
         <v>23</v>
       </c>
       <c r="F26" s="1">
-        <v>0.9103</v>
+        <v>0.94950999999999997</v>
       </c>
       <c r="G26" t="s">
         <v>23</v>
       </c>
       <c r="H26" s="1">
-        <v>0.89190000000000003</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.87021000000000004</v>
+      </c>
+      <c r="I26" t="s">
+        <v>23</v>
+      </c>
+      <c r="J26" s="1">
+        <v>0.77005999999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B27" s="1">
-        <v>0.92757999999999996</v>
+        <v>0.99761999999999995</v>
       </c>
       <c r="C27" t="s">
         <v>24</v>
       </c>
       <c r="D27" s="1">
-        <v>0.92625000000000002</v>
+        <v>0.98678999999999994</v>
       </c>
       <c r="E27" t="s">
         <v>24</v>
       </c>
       <c r="F27" s="1">
-        <v>0.86519999999999997</v>
+        <v>0.89941000000000004</v>
       </c>
       <c r="G27" t="s">
         <v>24</v>
       </c>
       <c r="H27" s="1">
-        <v>0.84165999999999996</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.81774999999999998</v>
+      </c>
+      <c r="I27" t="s">
+        <v>24</v>
+      </c>
+      <c r="J27" s="1">
+        <v>0.72374000000000005</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B28" s="1">
-        <v>0.98104999999999998</v>
+        <v>0.99914000000000003</v>
       </c>
       <c r="C28" t="s">
         <v>25</v>
       </c>
       <c r="D28" s="1">
-        <v>0.98141</v>
+        <v>0.99853999999999998</v>
       </c>
       <c r="E28" t="s">
         <v>25</v>
       </c>
       <c r="F28" s="1">
-        <v>0.98314000000000001</v>
+        <v>0.99365999999999999</v>
       </c>
       <c r="G28" t="s">
         <v>25</v>
       </c>
       <c r="H28" s="1">
-        <v>0.97943000000000002</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.97021000000000002</v>
+      </c>
+      <c r="I28" t="s">
+        <v>25</v>
+      </c>
+      <c r="J28" s="1">
+        <v>0.91576999999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B29" s="1">
-        <v>1.0008999999999999</v>
+        <v>0.99980999999999998</v>
       </c>
       <c r="C29" t="s">
         <v>26</v>
       </c>
       <c r="D29" s="1">
-        <v>0.99814000000000003</v>
+        <v>0.99875999999999998</v>
       </c>
       <c r="E29" t="s">
         <v>26</v>
       </c>
       <c r="F29" s="1">
-        <v>0.9627</v>
+        <v>0.96452000000000004</v>
       </c>
       <c r="G29" t="s">
         <v>26</v>
       </c>
       <c r="H29" s="1">
-        <v>0.93638999999999994</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.93418999999999996</v>
+      </c>
+      <c r="I29" t="s">
+        <v>26</v>
+      </c>
+      <c r="J29" s="1">
+        <v>0.86551</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B30" s="1">
-        <v>1.0402</v>
+        <v>1.0014000000000001</v>
       </c>
       <c r="C30" t="s">
         <v>27</v>
       </c>
       <c r="D30" s="1">
-        <v>1.0375000000000001</v>
+        <v>1.0045999999999999</v>
       </c>
       <c r="E30" t="s">
         <v>27</v>
       </c>
       <c r="F30" s="1">
-        <v>1.0183</v>
+        <v>0.99956</v>
       </c>
       <c r="G30" t="s">
         <v>27</v>
       </c>
       <c r="H30" s="1">
-        <v>0.99043999999999999</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1.008</v>
+      </c>
+      <c r="I30" t="s">
+        <v>27</v>
+      </c>
+      <c r="J30" s="1">
+        <v>0.98343000000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B31" s="1">
-        <v>0.98807</v>
+        <v>0.99912999999999996</v>
       </c>
       <c r="C31" t="s">
         <v>28</v>
       </c>
       <c r="D31" s="1">
-        <v>0.98607999999999996</v>
+        <v>0.99827999999999995</v>
       </c>
       <c r="E31" t="s">
         <v>28</v>
       </c>
       <c r="F31" s="1">
-        <v>0.96319999999999995</v>
+        <v>0.97174000000000005</v>
       </c>
       <c r="G31" t="s">
         <v>28</v>
       </c>
       <c r="H31" s="1">
-        <v>0.95482</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.94498000000000004</v>
+      </c>
+      <c r="I31" t="s">
+        <v>28</v>
+      </c>
+      <c r="J31" s="1">
+        <v>0.89856999999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B32" s="1">
-        <v>1.0306999999999999</v>
+        <v>1.0004</v>
       </c>
       <c r="C32" t="s">
         <v>29</v>
       </c>
       <c r="D32" s="1">
-        <v>1.0269999999999999</v>
+        <v>1.002</v>
       </c>
       <c r="E32" t="s">
         <v>29</v>
       </c>
       <c r="F32" s="1">
-        <v>0.98723000000000005</v>
+        <v>0.97352000000000005</v>
       </c>
       <c r="G32" t="s">
         <v>29</v>
       </c>
       <c r="H32" s="1">
-        <v>0.95462999999999998</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.96538999999999997</v>
+      </c>
+      <c r="I32" t="s">
+        <v>29</v>
+      </c>
+      <c r="J32" s="1">
+        <v>0.92059000000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B33" s="1">
-        <v>0.98643000000000003</v>
+        <v>0.99980999999999998</v>
       </c>
       <c r="C33" t="s">
         <v>30</v>
       </c>
       <c r="D33" s="1">
-        <v>0.98519999999999996</v>
+        <v>0.99804000000000004</v>
       </c>
       <c r="E33" t="s">
         <v>30</v>
       </c>
       <c r="F33" s="1">
-        <v>0.97138999999999998</v>
+        <v>0.98163</v>
       </c>
       <c r="G33" t="s">
         <v>30</v>
       </c>
       <c r="H33" s="1">
-        <v>0.95215000000000005</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.94701999999999997</v>
+      </c>
+      <c r="I33" t="s">
+        <v>30</v>
+      </c>
+      <c r="J33" s="1">
+        <v>0.88204000000000005</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B34" s="1">
-        <v>1.0306999999999999</v>
+        <v>1.0004</v>
       </c>
       <c r="C34" t="s">
         <v>31</v>
       </c>
       <c r="D34" s="1">
-        <v>1.0269999999999999</v>
+        <v>1.002</v>
       </c>
       <c r="E34" t="s">
         <v>31</v>
       </c>
       <c r="F34" s="1">
-        <v>0.98721999999999999</v>
+        <v>0.97350000000000003</v>
       </c>
       <c r="G34" t="s">
         <v>31</v>
       </c>
       <c r="H34" s="1">
-        <v>0.95464000000000004</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.96538999999999997</v>
+      </c>
+      <c r="I34" t="s">
+        <v>31</v>
+      </c>
+      <c r="J34" s="1">
+        <v>0.92059999999999997</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B35" s="1">
-        <v>0.86611000000000005</v>
+        <v>0.99253000000000002</v>
       </c>
       <c r="C35" t="s">
         <v>32</v>
       </c>
       <c r="D35" s="1">
-        <v>0.87021000000000004</v>
+        <v>0.97297</v>
       </c>
       <c r="E35" t="s">
         <v>32</v>
       </c>
       <c r="F35" s="1">
-        <v>0.84184999999999999</v>
+        <v>0.90437999999999996</v>
       </c>
       <c r="G35" t="s">
         <v>32</v>
       </c>
       <c r="H35" s="1">
-        <v>0.83211999999999997</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.80264999999999997</v>
+      </c>
+      <c r="I35" t="s">
+        <v>32</v>
+      </c>
+      <c r="J35" s="1">
+        <v>0.69655999999999996</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B36" s="1">
-        <v>0.86655000000000004</v>
+        <v>0.99302999999999997</v>
       </c>
       <c r="C36" t="s">
         <v>33</v>
       </c>
       <c r="D36" s="1">
-        <v>0.86714999999999998</v>
+        <v>0.96921999999999997</v>
       </c>
       <c r="E36" t="s">
         <v>33</v>
       </c>
       <c r="F36" s="1">
-        <v>0.76327</v>
+        <v>0.81316999999999995</v>
       </c>
       <c r="G36" t="s">
         <v>33</v>
       </c>
       <c r="H36" s="1">
-        <v>0.75310999999999995</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.72014</v>
+      </c>
+      <c r="I36" t="s">
+        <v>33</v>
+      </c>
+      <c r="J36" s="1">
+        <v>0.63675999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B37" s="1">
-        <v>0.98587999999999998</v>
+        <v>0.99934000000000001</v>
       </c>
       <c r="C37" t="s">
         <v>34</v>
       </c>
       <c r="D37" s="1">
-        <v>0.98348000000000002</v>
+        <v>0.99629000000000001</v>
       </c>
       <c r="E37" t="s">
         <v>34</v>
       </c>
       <c r="F37" s="1">
-        <v>0.94267000000000001</v>
+        <v>0.95111000000000001</v>
       </c>
       <c r="G37" t="s">
         <v>34</v>
       </c>
       <c r="H37" s="1">
-        <v>0.91705000000000003</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.91057999999999995</v>
+      </c>
+      <c r="I37" t="s">
+        <v>34</v>
+      </c>
+      <c r="J37" s="1">
+        <v>0.84523999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B38" s="1">
-        <v>1.0367</v>
+        <v>1.0013000000000001</v>
       </c>
       <c r="C38" t="s">
         <v>35</v>
       </c>
       <c r="D38" s="1">
-        <v>1.0342</v>
+        <v>1.0044</v>
       </c>
       <c r="E38" t="s">
         <v>35</v>
       </c>
       <c r="F38" s="1">
-        <v>1.0173000000000001</v>
+        <v>1.0011000000000001</v>
       </c>
       <c r="G38" t="s">
         <v>35</v>
       </c>
       <c r="H38" s="1">
-        <v>0.99187000000000003</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1.0067999999999999</v>
+      </c>
+      <c r="I38" t="s">
+        <v>35</v>
+      </c>
+      <c r="J38" s="1">
+        <v>0.97758</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B39" s="1">
-        <v>1.0313000000000001</v>
+        <v>1.0008999999999999</v>
       </c>
       <c r="C39" t="s">
         <v>36</v>
       </c>
       <c r="D39" s="1">
-        <v>1.0281</v>
+        <v>1.0025999999999999</v>
       </c>
       <c r="E39" t="s">
         <v>36</v>
       </c>
       <c r="F39" s="1">
-        <v>0.99550000000000005</v>
+        <v>0.98353999999999997</v>
       </c>
       <c r="G39" t="s">
         <v>36</v>
       </c>
       <c r="H39" s="1">
-        <v>0.96148999999999996</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.98436000000000001</v>
+      </c>
+      <c r="I39" t="s">
+        <v>36</v>
+      </c>
+      <c r="J39" s="1">
+        <v>1.7681999999999999E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B40" s="1">
-        <v>0.98482000000000003</v>
+        <v>0.99609999999999999</v>
       </c>
       <c r="C40" t="s">
         <v>37</v>
       </c>
       <c r="D40" s="1">
-        <v>0.98475999999999997</v>
+        <v>0.99409999999999998</v>
       </c>
       <c r="E40" t="s">
         <v>37</v>
       </c>
       <c r="F40" s="1">
-        <v>0.95936999999999995</v>
+        <v>0.96267999999999998</v>
       </c>
       <c r="G40" t="s">
         <v>37</v>
       </c>
       <c r="H40" s="1">
-        <v>0.94530999999999998</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.94367000000000001</v>
+      </c>
+      <c r="I40" t="s">
+        <v>37</v>
+      </c>
+      <c r="J40" s="1">
+        <v>0.92893999999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B41" s="1">
-        <v>1.0006999999999999</v>
+        <v>2.0652999999999999E-3</v>
       </c>
       <c r="C41" t="s">
         <v>38</v>
       </c>
       <c r="D41" s="1">
-        <v>0.99812999999999996</v>
+        <v>1.0001</v>
       </c>
       <c r="E41" t="s">
         <v>38</v>
       </c>
       <c r="F41" s="1">
-        <v>0.96619999999999995</v>
+        <v>0.97228999999999999</v>
       </c>
       <c r="G41" t="s">
         <v>38</v>
       </c>
       <c r="H41" s="1">
-        <v>0.94130000000000003</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.94020999999999999</v>
+      </c>
+      <c r="I41" t="s">
+        <v>38</v>
+      </c>
+      <c r="J41" s="1">
+        <v>1.6092</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B42" s="1">
-        <v>0.98875000000000002</v>
+        <v>0.99902999999999997</v>
       </c>
       <c r="C42" t="s">
         <v>39</v>
       </c>
       <c r="D42" s="1">
-        <v>0.98897999999999997</v>
+        <v>0.99931000000000003</v>
       </c>
       <c r="E42" t="s">
         <v>39</v>
       </c>
       <c r="F42" s="1">
-        <v>0.98868999999999996</v>
+        <v>0.99526000000000003</v>
       </c>
       <c r="G42" t="s">
         <v>39</v>
       </c>
       <c r="H42" s="1">
-        <v>0.98134999999999994</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0.97565000000000002</v>
+      </c>
+      <c r="I42" t="s">
+        <v>39</v>
+      </c>
+      <c r="J42" s="1">
+        <v>0.90580000000000005</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B43" s="1">
-        <v>0.99334999999999996</v>
+        <v>0.99902999999999997</v>
       </c>
       <c r="C43" t="s">
         <v>40</v>
       </c>
       <c r="D43" s="1">
-        <v>0.99124999999999996</v>
+        <v>0.99861</v>
       </c>
       <c r="E43" t="s">
         <v>40</v>
       </c>
       <c r="F43" s="1">
-        <v>0.96555000000000002</v>
+        <v>0.97104000000000001</v>
       </c>
       <c r="G43" t="s">
         <v>40</v>
       </c>
       <c r="H43" s="1">
-        <v>0.95391000000000004</v>
+        <v>0.94696999999999998</v>
+      </c>
+      <c r="I43" t="s">
+        <v>40</v>
+      </c>
+      <c r="J43" s="1">
+        <v>0.89073000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
increase number of l-mixed levels to predict all lines
We need to l-resolve all levels for which we wish
to report nl-n'l' lines.   This increases the number of
resolved levels to do so.
</commit_message>
<xml_diff>
--- a/tsuite/experimental/he1nnt4.xlsx
+++ b/tsuite/experimental/he1nnt4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gary/cloudy/branches/CaseB22/tsuite/experimental/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87EABD8-F695-D042-AC3D-6ED08BBBEAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C025D92-9A24-F34F-B506-6F6DA2EA99B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12500" yWindow="5320" windowWidth="27640" windowHeight="16940" xr2:uid="{8843D32E-1EA8-8F49-A1DE-0F59999A652D}"/>
+    <workbookView xWindow="20520" yWindow="6200" windowWidth="27640" windowHeight="16940" xr2:uid="{8843D32E-1EA8-8F49-A1DE-0F59999A652D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -610,7 +610,7 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -619,7 +619,7 @@
     <col min="3" max="3" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -714,7 +714,7 @@
         <v>1</v>
       </c>
       <c r="J4" s="1">
-        <v>0.97755999999999998</v>
+        <v>0.93506</v>
       </c>
       <c r="K4" t="s">
         <v>47</v>
@@ -749,7 +749,7 @@
         <v>2</v>
       </c>
       <c r="J5" s="1">
-        <v>0.92247000000000001</v>
+        <v>0.89353000000000005</v>
       </c>
       <c r="K5" t="s">
         <v>48</v>
@@ -784,7 +784,7 @@
         <v>3</v>
       </c>
       <c r="J6" s="1">
-        <v>0.95409999999999995</v>
+        <v>0.92720999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -816,7 +816,7 @@
         <v>4</v>
       </c>
       <c r="J7" s="1">
-        <v>0.92059000000000002</v>
+        <v>0.89563000000000004</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -848,7 +848,7 @@
         <v>5</v>
       </c>
       <c r="J8" s="1">
-        <v>0.90178999999999998</v>
+        <v>0.92318999999999996</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -880,7 +880,7 @@
         <v>6</v>
       </c>
       <c r="J9" s="1">
-        <v>0.91574999999999995</v>
+        <v>0.93901999999999997</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -912,7 +912,7 @@
         <v>7</v>
       </c>
       <c r="J10" s="1">
-        <v>0.86551999999999996</v>
+        <v>0.87756000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -944,7 +944,7 @@
         <v>8</v>
       </c>
       <c r="J11" s="1">
-        <v>0.89856999999999998</v>
+        <v>0.93145999999999995</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -976,7 +976,7 @@
         <v>9</v>
       </c>
       <c r="J12" s="11">
-        <v>0.88202999999999998</v>
+        <v>0.90483000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -1008,7 +1008,7 @@
         <v>10</v>
       </c>
       <c r="J13" s="1">
-        <v>0.90586999999999995</v>
+        <v>0.92825000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -1040,7 +1040,7 @@
         <v>11</v>
       </c>
       <c r="J14" s="1">
-        <v>0.84523999999999999</v>
+        <v>0.86412999999999995</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -1072,7 +1072,7 @@
         <v>12</v>
       </c>
       <c r="J15" s="1">
-        <v>0.91208999999999996</v>
+        <v>0.89712000000000003</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -1104,7 +1104,7 @@
         <v>13</v>
       </c>
       <c r="J16" s="1">
-        <v>0.89078000000000002</v>
+        <v>0.91886999999999996</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -1136,7 +1136,7 @@
         <v>14</v>
       </c>
       <c r="J17" s="11">
-        <v>0.82025999999999999</v>
+        <v>0.85948000000000002</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -1168,7 +1168,7 @@
         <v>15</v>
       </c>
       <c r="J18" s="11">
-        <v>0.78088000000000002</v>
+        <v>0.81681999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -1200,7 +1200,7 @@
         <v>16</v>
       </c>
       <c r="J19" s="1">
-        <v>0.90383999999999998</v>
+        <v>0.90776000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -1232,7 +1232,7 @@
         <v>17</v>
       </c>
       <c r="J20" s="1">
-        <v>0.90114000000000005</v>
+        <v>0.91281999999999996</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -1264,7 +1264,7 @@
         <v>18</v>
       </c>
       <c r="J21" s="1">
-        <v>0.98345000000000005</v>
+        <v>0.93188000000000004</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -1296,7 +1296,7 @@
         <v>19</v>
       </c>
       <c r="J22" s="14">
-        <v>0.43336000000000002</v>
+        <v>0.43247000000000002</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -1328,7 +1328,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="1">
-        <v>0.92245999999999995</v>
+        <v>0.89351999999999998</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -1360,7 +1360,7 @@
         <v>21</v>
       </c>
       <c r="J24" s="1">
-        <v>0.90178999999999998</v>
+        <v>0.92318</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -1392,7 +1392,7 @@
         <v>22</v>
       </c>
       <c r="J25" s="1">
-        <v>0.97755999999999998</v>
+        <v>0.93506</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -1424,7 +1424,7 @@
         <v>23</v>
       </c>
       <c r="J26" s="1">
-        <v>0.77005999999999997</v>
+        <v>0.83423999999999998</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
@@ -1456,7 +1456,7 @@
         <v>24</v>
       </c>
       <c r="J27" s="1">
-        <v>0.72374000000000005</v>
+        <v>0.78149999999999997</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -1488,7 +1488,7 @@
         <v>25</v>
       </c>
       <c r="J28" s="1">
-        <v>0.91576999999999997</v>
+        <v>0.93903999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
@@ -1520,7 +1520,7 @@
         <v>26</v>
       </c>
       <c r="J29" s="1">
-        <v>0.86551</v>
+        <v>0.87756000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
@@ -1552,7 +1552,7 @@
         <v>27</v>
       </c>
       <c r="J30" s="1">
-        <v>0.98343000000000003</v>
+        <v>0.93186999999999998</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
@@ -1584,7 +1584,7 @@
         <v>28</v>
       </c>
       <c r="J31" s="1">
-        <v>0.89856999999999998</v>
+        <v>0.93147000000000002</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
@@ -1616,7 +1616,7 @@
         <v>29</v>
       </c>
       <c r="J32" s="1">
-        <v>0.92059000000000002</v>
+        <v>0.89563000000000004</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
@@ -1648,7 +1648,7 @@
         <v>30</v>
       </c>
       <c r="J33" s="1">
-        <v>0.88204000000000005</v>
+        <v>0.90483999999999998</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
@@ -1680,7 +1680,7 @@
         <v>31</v>
       </c>
       <c r="J34" s="1">
-        <v>0.92059999999999997</v>
+        <v>0.89563999999999999</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
@@ -1712,7 +1712,7 @@
         <v>32</v>
       </c>
       <c r="J35" s="1">
-        <v>0.69655999999999996</v>
+        <v>0.78283999999999998</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
@@ -1744,7 +1744,7 @@
         <v>33</v>
       </c>
       <c r="J36" s="1">
-        <v>0.63675999999999999</v>
+        <v>0.71048</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
@@ -1776,7 +1776,7 @@
         <v>34</v>
       </c>
       <c r="J37" s="1">
-        <v>0.84523999999999999</v>
+        <v>0.86414000000000002</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
@@ -1808,7 +1808,7 @@
         <v>35</v>
       </c>
       <c r="J38" s="1">
-        <v>0.97758</v>
+        <v>0.93506999999999996</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
@@ -1840,7 +1840,7 @@
         <v>36</v>
       </c>
       <c r="J39" s="1">
-        <v>1.7681999999999999E-3</v>
+        <v>0.87392999999999998</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
@@ -1872,7 +1872,7 @@
         <v>37</v>
       </c>
       <c r="J40" s="1">
-        <v>0.92893999999999999</v>
+        <v>0.92986000000000002</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
@@ -1904,7 +1904,7 @@
         <v>38</v>
       </c>
       <c r="J41" s="1">
-        <v>1.6092</v>
+        <v>0.88553000000000004</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
@@ -1936,7 +1936,7 @@
         <v>39</v>
       </c>
       <c r="J42" s="1">
-        <v>0.90580000000000005</v>
+        <v>0.92818999999999996</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
@@ -1968,7 +1968,7 @@
         <v>40</v>
       </c>
       <c r="J43" s="1">
-        <v>0.89073000000000002</v>
+        <v>0.91883000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>